<commit_message>
habia dejado ws y ts mal en los titulares, entonces no unia bien
</commit_message>
<xml_diff>
--- a/preguntas/estructura/2021.xlsx
+++ b/preguntas/estructura/2021.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="223">
   <si>
     <t xml:space="preserve">T</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t xml:space="preserve">Subpregunta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ws</t>
   </si>
   <si>
     <t xml:space="preserve">IIP2021</t>
@@ -780,7 +786,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -821,16 +827,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -970,8 +968,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36:M37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="15.1" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,39 +1019,39 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="114.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J2" s="7" t="n">
         <v>0</v>
@@ -1064,31 +1062,31 @@
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>4</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J3" s="7" t="n">
         <v>4</v>
@@ -1099,31 +1097,31 @@
     </row>
     <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>7.7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J4" s="7" t="n">
         <v>1</v>
@@ -1134,31 +1132,31 @@
     </row>
     <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>7.7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J5" s="9" t="n">
         <v>3</v>
@@ -1169,31 +1167,31 @@
     </row>
     <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E6" s="6" t="n">
         <v>7.7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G6" s="7" t="n">
         <v>3.7</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J6" s="7" t="n">
         <v>1</v>
@@ -1204,31 +1202,31 @@
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>7.7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="n">
         <v>3.7</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J7" s="9" t="n">
         <v>2.7</v>
@@ -1239,31 +1237,31 @@
     </row>
     <row r="8" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E8" s="6" t="n">
         <v>8.7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" s="7" t="n">
         <v>4.7</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J8" s="7" t="n">
         <v>2</v>
@@ -1274,31 +1272,31 @@
     </row>
     <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="6" t="n">
         <v>8.7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="7" t="n">
         <v>4.7</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J9" s="9" t="n">
         <v>2.7</v>
@@ -1309,31 +1307,31 @@
     </row>
     <row r="10" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="6" t="n">
         <v>8.7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G10" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J10" s="7" t="n">
         <v>1.5</v>
@@ -1344,31 +1342,31 @@
     </row>
     <row r="11" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="6" t="n">
         <v>8.7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G11" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J11" s="9" t="n">
         <v>2.5</v>
@@ -1379,31 +1377,31 @@
     </row>
     <row r="12" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12" s="6" t="n">
         <v>4.6</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G12" s="7" t="n">
         <v>4.6</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J12" s="7" t="n">
         <v>2.1</v>
@@ -1414,31 +1412,31 @@
     </row>
     <row r="13" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E13" s="6" t="n">
         <v>4.6</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G13" s="7" t="n">
         <v>4.6</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J13" s="7" t="n">
         <v>1</v>
@@ -1449,31 +1447,31 @@
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" s="6" t="n">
         <v>4.6</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G14" s="7" t="n">
         <v>4.6</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J14" s="7" t="n">
         <v>1.5</v>
@@ -1484,66 +1482,66 @@
     </row>
     <row r="15" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E15" s="9" t="n">
         <v>9</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="11" t="n">
+        <v>43</v>
+      </c>
+      <c r="G15" s="10" t="n">
         <v>2.8</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="J15" s="10" t="n">
         <v>2.8</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="11"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E16" s="9" t="n">
         <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J16" s="9" t="n">
         <v>1</v>
@@ -1554,40 +1552,40 @@
     </row>
     <row r="17" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E17" s="9" t="n">
         <v>9</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>2.8</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J17" s="9" t="n">
         <v>2.8</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M17" s="9" t="n">
         <v>2.8</v>
@@ -1595,31 +1593,31 @@
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="10" t="n">
+        <v>42</v>
+      </c>
+      <c r="E18" s="9" t="n">
         <v>9</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G18" s="9" t="n">
         <v>2.4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J18" s="9" t="n">
         <v>2.4</v>
@@ -1630,40 +1628,40 @@
     </row>
     <row r="19" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E19" s="6" t="n">
         <v>8</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G19" s="7" t="n">
         <v>3</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J19" s="7" t="n">
         <v>3</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M19" s="7" t="n">
         <v>3</v>
@@ -1671,40 +1669,40 @@
     </row>
     <row r="20" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6" t="n">
         <v>8</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>3</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J20" s="9" t="n">
         <v>3</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M20" s="9" t="n">
         <v>3</v>
@@ -1712,31 +1710,31 @@
     </row>
     <row r="21" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E21" s="6" t="n">
         <v>8</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G21" s="7" t="n">
         <v>2</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J21" s="7" t="n">
         <v>2</v>
@@ -1744,44 +1742,44 @@
       <c r="K21" s="5"/>
       <c r="L21" s="8"/>
       <c r="M21" s="7"/>
-      <c r="O21" s="12"/>
+      <c r="O21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E22" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G22" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J22" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M22" s="9" t="n">
         <v>1.4</v>
@@ -1789,40 +1787,40 @@
     </row>
     <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E23" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G23" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J23" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M23" s="9" t="n">
         <v>1.4</v>
@@ -1830,40 +1828,40 @@
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E24" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G24" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J24" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M24" s="9" t="n">
         <v>0</v>
@@ -1871,40 +1869,40 @@
     </row>
     <row r="25" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C25" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E25" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G25" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J25" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M25" s="9" t="n">
         <v>0</v>
@@ -1912,40 +1910,40 @@
     </row>
     <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E26" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G26" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J26" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M26" s="9" t="n">
         <v>0</v>
@@ -1953,40 +1951,40 @@
     </row>
     <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E27" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G27" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J27" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M27" s="9" t="n">
         <v>1.4</v>
@@ -1994,40 +1992,40 @@
     </row>
     <row r="28" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E28" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G28" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J28" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M28" s="9" t="n">
         <v>1.4</v>
@@ -2035,40 +2033,40 @@
     </row>
     <row r="29" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E29" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G29" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J29" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M29" s="9" t="n">
         <v>1.4</v>
@@ -2076,40 +2074,40 @@
     </row>
     <row r="30" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C30" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E30" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G30" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J30" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M30" s="9" t="n">
         <v>0</v>
@@ -2117,40 +2115,40 @@
     </row>
     <row r="31" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C31" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E31" s="6" t="n">
         <v>7</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G31" s="9" t="n">
         <v>7</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J31" s="9" t="n">
         <v>7</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M31" s="9" t="n">
         <v>0</v>
@@ -2158,31 +2156,31 @@
     </row>
     <row r="32" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E32" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G32" s="9" t="n">
         <v>6</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J32" s="9" t="n">
         <v>6</v>
@@ -2193,31 +2191,31 @@
     </row>
     <row r="33" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E33" s="6" t="n">
         <v>5</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G33" s="9" t="n">
         <v>2.8</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J33" s="9" t="n">
         <v>2.8</v>
@@ -2228,31 +2226,31 @@
     </row>
     <row r="34" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E34" s="6" t="n">
         <v>5</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G34" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J34" s="9" t="n">
         <v>1.1</v>
@@ -2263,31 +2261,31 @@
     </row>
     <row r="35" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C35" s="6" t="n">
         <v>35</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E35" s="6" t="n">
         <v>5</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G35" s="9" t="n">
         <v>1.1</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J35" s="9" t="n">
         <v>1.1</v>
@@ -2298,40 +2296,40 @@
     </row>
     <row r="36" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C36" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E36" s="6" t="n">
         <v>17</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G36" s="7" t="n">
         <v>17</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J36" s="7" t="n">
         <v>17</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M36" s="7" t="n">
         <v>8.5</v>
@@ -2339,40 +2337,40 @@
     </row>
     <row r="37" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C37" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E37" s="6" t="n">
         <v>17</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G37" s="7" t="n">
         <v>17</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J37" s="7" t="n">
         <v>17</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M37" s="7" t="n">
         <v>8.5</v>
@@ -2380,31 +2378,31 @@
     </row>
     <row r="38" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C38" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E38" s="6" t="n">
         <v>2</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G38" s="9" t="n">
         <v>1</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J38" s="9" t="n">
         <v>1</v>
@@ -2415,31 +2413,31 @@
     </row>
     <row r="39" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C39" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E39" s="6" t="n">
         <v>2</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G39" s="9" t="n">
         <v>1</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J39" s="9" t="n">
         <v>1</v>
@@ -2450,31 +2448,31 @@
     </row>
     <row r="40" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C40" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E40" s="6" t="n">
         <v>1.5</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G40" s="9" t="n">
         <v>1.5</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J40" s="9" t="n">
         <v>1.5</v>
@@ -2485,31 +2483,31 @@
     </row>
     <row r="41" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E41" s="6" t="n">
         <v>4.5</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G41" s="7" t="n">
         <v>2.2</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J41" s="7" t="n">
         <v>2.2</v>
@@ -2520,31 +2518,31 @@
     </row>
     <row r="42" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E42" s="6" t="n">
         <v>4.5</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G42" s="9" t="n">
         <v>2.3</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J42" s="9" t="n">
         <v>2.3</v>
@@ -2555,31 +2553,31 @@
     </row>
     <row r="43" customFormat="false" ht="100.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C43" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E43" s="6" t="n">
         <v>3</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G43" s="9" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J43" s="9" t="n">
         <v>0</v>
@@ -2590,31 +2588,31 @@
     </row>
     <row r="44" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C44" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E44" s="6" t="n">
         <v>3</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G44" s="9" t="n">
         <v>3</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J44" s="9" t="n">
         <v>3</v>
@@ -2625,31 +2623,31 @@
     </row>
     <row r="45" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C45" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E45" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G45" s="7" t="n">
         <v>1.2</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J45" s="7" t="n">
         <v>1.2</v>
@@ -2660,31 +2658,31 @@
     </row>
     <row r="46" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C46" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E46" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G46" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J46" s="9" t="n">
         <v>0.96</v>
@@ -2695,31 +2693,31 @@
     </row>
     <row r="47" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C47" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E47" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G47" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J47" s="9" t="n">
         <v>0.96</v>
@@ -2730,31 +2728,31 @@
     </row>
     <row r="48" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C48" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E48" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G48" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J48" s="9" t="n">
         <v>0.96</v>
@@ -2765,40 +2763,40 @@
     </row>
     <row r="49" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C49" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E49" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J49" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M49" s="9" t="n">
         <v>0.96</v>
@@ -2806,40 +2804,40 @@
     </row>
     <row r="50" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C50" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E50" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G50" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J50" s="9" t="n">
         <v>0.96</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M50" s="9" t="n">
         <v>0.96</v>
@@ -2847,31 +2845,31 @@
     </row>
     <row r="51" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C51" s="6" t="n">
         <v>15</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E51" s="6" t="n">
         <v>6</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G51" s="9" t="n">
         <v>4</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J51" s="9" t="n">
         <v>6</v>
@@ -2881,19 +2879,19 @@
       <c r="M51" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J53" s="13"/>
+      <c r="J53" s="11"/>
     </row>
     <row r="65" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J65" s="13"/>
+      <c r="J65" s="11"/>
     </row>
     <row r="70" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J70" s="14"/>
+      <c r="J70" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J72" s="14"/>
+      <c r="J72" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J74" s="14"/>
+      <c r="J74" s="12"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2916,7 +2914,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="M36:M37 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="15.1" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2924,7 +2922,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="13" width="9.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="11" width="9.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2940,556 +2938,556 @@
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>126</v>
+      <c r="E1" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="114.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>22</v>
+      <c r="C2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>22</v>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>22</v>
+      <c r="C4" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>22</v>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>22</v>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>22</v>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>22</v>
+      <c r="C8" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>22</v>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>22</v>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>22</v>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" s="15" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>22</v>
+      <c r="C12" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>22</v>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>22</v>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>22</v>
+      <c r="C15" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>22</v>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>22</v>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>22</v>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="15" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>22</v>
+      <c r="C19" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>22</v>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>22</v>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>22</v>
+      <c r="C22" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>22</v>
+      <c r="C23" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>22</v>
+      <c r="C24" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>22</v>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>22</v>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C27" s="15" t="s">
+      <c r="A27" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>22</v>
+      <c r="C27" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D28" s="15" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>22</v>
+      <c r="C28" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>22</v>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>22</v>
+      <c r="C30" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="D31" s="15" t="s">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>22</v>
+      <c r="C31" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>22</v>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="100.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="A33" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="B33" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>22</v>
+      <c r="C33" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>22</v>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="D35" s="15" t="s">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>22</v>
+      <c r="C35" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>22</v>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>22</v>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>22</v>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>22</v>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>22</v>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D41" s="15" t="s">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>22</v>
+      <c r="C41" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>